<commit_message>
updated xlsx age gender
</commit_message>
<xml_diff>
--- a/excels/lite/lite-Ages-Gender.xlsx
+++ b/excels/lite/lite-Ages-Gender.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16100" xWindow="240" yWindow="460"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="31280" windowHeight="14480"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" concurrentCalc="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -59,34 +64,24 @@
   </si>
   <si>
     <t>M.65+</t>
-  </si>
-  <si>
-    <t>13-02-2019</t>
-  </si>
-  <si>
-    <t>14-02-2019</t>
-  </si>
-  <si>
-    <t>16-02-2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,16 +97,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -399,20 +395,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="10"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -463,570 +455,575 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="1">
         <v>43499</v>
       </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
         <v>42</v>
       </c>
-      <c r="D2" t="n">
-        <v>49</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2">
+        <v>49</v>
+      </c>
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>34</v>
       </c>
-      <c r="G2" t="n">
-        <v>11</v>
-      </c>
-      <c r="H2" t="n">
-        <v>4</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="G2">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>75</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>20</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>20</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>17</v>
       </c>
-      <c r="N2" t="n">
-        <v>11</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="N2">
+        <v>11</v>
+      </c>
+      <c r="O2">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="1">
         <v>43501</v>
       </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>45</v>
       </c>
-      <c r="D3" t="n">
-        <v>49</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3">
+        <v>49</v>
+      </c>
+      <c r="E3">
         <v>31</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>37</v>
       </c>
-      <c r="G3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>76</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3">
         <v>20</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3">
         <v>20</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3">
         <v>18</v>
       </c>
-      <c r="N3" t="n">
-        <v>11</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="N3">
+        <v>11</v>
+      </c>
+      <c r="O3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="1">
         <v>43503</v>
       </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>51</v>
       </c>
-      <c r="D4" t="n">
-        <v>49</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
+        <v>49</v>
+      </c>
+      <c r="E4">
         <v>31</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>35</v>
       </c>
-      <c r="G4" t="n">
-        <v>11</v>
-      </c>
-      <c r="H4" t="n">
-        <v>4</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>77</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4">
         <v>22</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4">
         <v>21</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4">
         <v>19</v>
       </c>
-      <c r="N4" t="n">
-        <v>11</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="N4">
+        <v>11</v>
+      </c>
+      <c r="O4">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="1">
         <v>43504</v>
       </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>51</v>
       </c>
-      <c r="D5" t="n">
-        <v>49</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="D5">
+        <v>49</v>
+      </c>
+      <c r="E5">
         <v>32</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>37</v>
       </c>
-      <c r="G5" t="n">
-        <v>11</v>
-      </c>
-      <c r="H5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="G5">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>78</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5">
         <v>25</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5">
         <v>22</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5">
         <v>19</v>
       </c>
-      <c r="N5" t="n">
-        <v>11</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="N5">
+        <v>11</v>
+      </c>
+      <c r="O5">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="1">
         <v>43505</v>
       </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>51</v>
       </c>
-      <c r="D6" t="n">
-        <v>49</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="D6">
+        <v>49</v>
+      </c>
+      <c r="E6">
         <v>32</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>37</v>
       </c>
-      <c r="G6" t="n">
-        <v>11</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="n">
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>78</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6">
         <v>25</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6">
         <v>24</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6">
         <v>19</v>
       </c>
-      <c r="N6" t="n">
-        <v>11</v>
-      </c>
-      <c r="O6" t="n">
+      <c r="N6">
+        <v>11</v>
+      </c>
+      <c r="O6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="1">
         <v>43507</v>
       </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
         <v>51</v>
       </c>
-      <c r="D7" t="n">
-        <v>49</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="D7">
+        <v>49</v>
+      </c>
+      <c r="E7">
         <v>32</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>37</v>
       </c>
-      <c r="G7" t="n">
-        <v>11</v>
-      </c>
-      <c r="H7" t="n">
-        <v>4</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
         <v>78</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7">
         <v>25</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L7">
         <v>24</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M7">
         <v>19</v>
       </c>
-      <c r="N7" t="n">
-        <v>11</v>
-      </c>
-      <c r="O7" t="n">
+      <c r="N7">
+        <v>11</v>
+      </c>
+      <c r="O7">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="1">
         <v>43507</v>
       </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
         <v>51</v>
       </c>
-      <c r="D8" t="n">
-        <v>49</v>
-      </c>
-      <c r="E8" t="n">
+      <c r="D8">
+        <v>49</v>
+      </c>
+      <c r="E8">
         <v>32</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>37</v>
       </c>
-      <c r="G8" t="n">
-        <v>11</v>
-      </c>
-      <c r="H8" t="n">
-        <v>4</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" t="n">
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
         <v>78</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8">
         <v>25</v>
       </c>
-      <c r="L8" t="n">
+      <c r="L8">
         <v>24</v>
       </c>
-      <c r="M8" t="n">
+      <c r="M8">
         <v>19</v>
       </c>
-      <c r="N8" t="n">
-        <v>11</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="N8">
+        <v>11</v>
+      </c>
+      <c r="O8">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="1">
         <v>43507</v>
       </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
         <v>51</v>
       </c>
-      <c r="D9" t="n">
-        <v>49</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="D9">
+        <v>49</v>
+      </c>
+      <c r="E9">
         <v>32</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>37</v>
       </c>
-      <c r="G9" t="n">
-        <v>11</v>
-      </c>
-      <c r="H9" t="n">
-        <v>4</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
+      <c r="G9">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>78</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9">
         <v>25</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L9">
         <v>24</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M9">
         <v>19</v>
       </c>
-      <c r="N9" t="n">
-        <v>11</v>
-      </c>
-      <c r="O9" t="n">
+      <c r="N9">
+        <v>11</v>
+      </c>
+      <c r="O9">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="1">
         <v>43508</v>
       </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
         <v>51</v>
       </c>
-      <c r="D10" t="n">
-        <v>49</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="D10">
+        <v>49</v>
+      </c>
+      <c r="E10">
         <v>32</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>37</v>
       </c>
-      <c r="G10" t="n">
-        <v>11</v>
-      </c>
-      <c r="H10" t="n">
-        <v>4</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" t="n">
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
         <v>78</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10">
         <v>25</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L10">
         <v>24</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10">
         <v>19</v>
       </c>
-      <c r="N10" t="n">
-        <v>11</v>
-      </c>
-      <c r="O10" t="n">
+      <c r="N10">
+        <v>11</v>
+      </c>
+      <c r="O10">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="n">
+      <c r="A11" s="1">
+        <v>43509</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
         <v>51</v>
       </c>
-      <c r="D11" t="n">
-        <v>49</v>
-      </c>
-      <c r="E11" t="n">
+      <c r="D11">
+        <v>49</v>
+      </c>
+      <c r="E11">
         <v>32</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>37</v>
       </c>
-      <c r="G11" t="n">
-        <v>11</v>
-      </c>
-      <c r="H11" t="n">
-        <v>4</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" t="n">
+      <c r="G11">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
         <v>78</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K11">
         <v>25</v>
       </c>
-      <c r="L11" t="n">
+      <c r="L11">
         <v>24</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M11">
         <v>19</v>
       </c>
-      <c r="N11" t="n">
-        <v>11</v>
-      </c>
-      <c r="O11" t="n">
+      <c r="N11">
+        <v>11</v>
+      </c>
+      <c r="O11">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="n">
+      <c r="A12" s="1">
+        <v>43510</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
         <v>51</v>
       </c>
-      <c r="D12" t="n">
-        <v>49</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="D12">
+        <v>49</v>
+      </c>
+      <c r="E12">
         <v>32</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>36</v>
       </c>
-      <c r="G12" t="n">
-        <v>11</v>
-      </c>
-      <c r="H12" t="n">
-        <v>4</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" t="n">
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
         <v>78</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K12">
         <v>25</v>
       </c>
-      <c r="L12" t="n">
+      <c r="L12">
         <v>24</v>
       </c>
-      <c r="M12" t="n">
+      <c r="M12">
         <v>19</v>
       </c>
-      <c r="N12" t="n">
-        <v>11</v>
-      </c>
-      <c r="O12" t="n">
+      <c r="N12">
+        <v>11</v>
+      </c>
+      <c r="O12">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="n">
+      <c r="A13" s="1">
+        <v>43512</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
         <v>51</v>
       </c>
-      <c r="D13" t="n">
-        <v>49</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="D13">
+        <v>49</v>
+      </c>
+      <c r="E13">
         <v>32</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>36</v>
       </c>
-      <c r="G13" t="n">
-        <v>11</v>
-      </c>
-      <c r="H13" t="n">
-        <v>4</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" t="n">
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
         <v>78</v>
       </c>
-      <c r="K13" t="n">
+      <c r="K13">
         <v>25</v>
       </c>
-      <c r="L13" t="n">
+      <c r="L13">
         <v>24</v>
       </c>
-      <c r="M13" t="n">
+      <c r="M13">
         <v>19</v>
       </c>
-      <c r="N13" t="n">
-        <v>11</v>
-      </c>
-      <c r="O13" t="n">
+      <c r="N13">
+        <v>11</v>
+      </c>
+      <c r="O13">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working age group targeting
</commit_message>
<xml_diff>
--- a/excels/lite/lite-Ages-Gender.xlsx
+++ b/excels/lite/lite-Ages-Gender.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgosandreou/Documents/Visual Studio/thesis-old/excels/lite/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="5260" windowWidth="31280" windowHeight="14480"/>
+    <workbookView xWindow="3640" yWindow="5680" windowWidth="33020" windowHeight="14480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,6 +142,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -425,18 +435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43499</v>
       </c>
@@ -530,7 +540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43501</v>
       </c>
@@ -577,7 +587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43503</v>
       </c>
@@ -624,7 +634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43504</v>
       </c>
@@ -671,7 +681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43505</v>
       </c>
@@ -718,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43507</v>
       </c>
@@ -765,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43507</v>
       </c>
@@ -812,7 +822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43507</v>
       </c>
@@ -859,7 +869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43508</v>
       </c>
@@ -906,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43509</v>
       </c>
@@ -953,7 +963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43510</v>
       </c>
@@ -1000,7 +1010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43512</v>
       </c>
@@ -1047,7 +1057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43515</v>
       </c>
@@ -1094,7 +1104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43519</v>
       </c>
@@ -1141,7 +1151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43520</v>
       </c>
@@ -1188,7 +1198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43521</v>
       </c>
@@ -1235,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43525</v>
       </c>
@@ -1282,7 +1292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43526</v>
       </c>
@@ -1329,7 +1339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43527</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43528</v>
       </c>
@@ -1423,7 +1433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43529</v>
       </c>
@@ -1470,7 +1480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43530</v>
       </c>
@@ -1517,7 +1527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43531</v>
       </c>
@@ -1564,7 +1574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43532</v>
       </c>
@@ -1611,7 +1621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43533</v>
       </c>
@@ -1658,7 +1668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43534</v>
       </c>
@@ -1705,7 +1715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43535</v>
       </c>
@@ -1752,7 +1762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43536</v>
       </c>
@@ -1799,7 +1809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43537</v>
       </c>
@@ -1846,7 +1856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43538</v>
       </c>
@@ -1893,7 +1903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43539</v>
       </c>
@@ -1940,7 +1950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43540</v>
       </c>
@@ -1987,7 +1997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43541</v>
       </c>
@@ -2034,7 +2044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43542</v>
       </c>
@@ -2081,7 +2091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43543</v>
       </c>
@@ -2128,7 +2138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43544</v>
       </c>
@@ -2175,9 +2185,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43548</v>
+        <v>43545</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -2222,9 +2232,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43549</v>
+        <v>43546</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -2269,9 +2279,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43550</v>
+        <v>43547</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -2316,9 +2326,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43554</v>
+        <v>43548</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -2336,7 +2346,7 @@
         <v>36</v>
       </c>
       <c r="G41">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H41">
         <v>4</v>
@@ -2351,10 +2361,10 @@
         <v>27</v>
       </c>
       <c r="L41">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M41">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N41">
         <v>11</v>
@@ -2363,9 +2373,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43556</v>
+        <v>43549</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -2383,275 +2393,599 @@
         <v>36</v>
       </c>
       <c r="G42">
+        <v>11</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>75</v>
+      </c>
+      <c r="K42">
+        <v>27</v>
+      </c>
+      <c r="L42">
+        <v>23</v>
+      </c>
+      <c r="M42">
+        <v>19</v>
+      </c>
+      <c r="N42">
+        <v>11</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>43550</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>50</v>
+      </c>
+      <c r="D43">
+        <v>48</v>
+      </c>
+      <c r="E43">
+        <v>34</v>
+      </c>
+      <c r="F43">
+        <v>36</v>
+      </c>
+      <c r="G43">
+        <v>11</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>75</v>
+      </c>
+      <c r="K43">
+        <v>27</v>
+      </c>
+      <c r="L43">
+        <v>23</v>
+      </c>
+      <c r="M43">
+        <v>19</v>
+      </c>
+      <c r="N43">
+        <v>11</v>
+      </c>
+      <c r="O43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>43551</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>50</v>
+      </c>
+      <c r="D44">
+        <v>48</v>
+      </c>
+      <c r="E44">
+        <v>34</v>
+      </c>
+      <c r="F44">
+        <v>36</v>
+      </c>
+      <c r="G44">
+        <v>11</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>75</v>
+      </c>
+      <c r="K44">
+        <v>27</v>
+      </c>
+      <c r="L44">
+        <v>23</v>
+      </c>
+      <c r="M44">
+        <v>19</v>
+      </c>
+      <c r="N44">
+        <v>11</v>
+      </c>
+      <c r="O44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>43552</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>50</v>
+      </c>
+      <c r="D45">
+        <v>48</v>
+      </c>
+      <c r="E45">
+        <v>34</v>
+      </c>
+      <c r="F45">
+        <v>36</v>
+      </c>
+      <c r="G45">
+        <v>11</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>75</v>
+      </c>
+      <c r="K45">
+        <v>27</v>
+      </c>
+      <c r="L45">
+        <v>23</v>
+      </c>
+      <c r="M45">
+        <v>19</v>
+      </c>
+      <c r="N45">
+        <v>11</v>
+      </c>
+      <c r="O45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>43553</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>50</v>
+      </c>
+      <c r="D46">
+        <v>48</v>
+      </c>
+      <c r="E46">
+        <v>34</v>
+      </c>
+      <c r="F46">
+        <v>36</v>
+      </c>
+      <c r="G46">
+        <v>11</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>75</v>
+      </c>
+      <c r="K46">
+        <v>27</v>
+      </c>
+      <c r="L46">
+        <v>23</v>
+      </c>
+      <c r="M46">
+        <v>19</v>
+      </c>
+      <c r="N46">
+        <v>11</v>
+      </c>
+      <c r="O46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>43554</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>50</v>
+      </c>
+      <c r="D47">
+        <v>48</v>
+      </c>
+      <c r="E47">
+        <v>34</v>
+      </c>
+      <c r="F47">
+        <v>36</v>
+      </c>
+      <c r="G47">
         <v>12</v>
       </c>
-      <c r="H42">
-        <v>4</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
+      <c r="H47">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>75</v>
+      </c>
+      <c r="K47">
+        <v>27</v>
+      </c>
+      <c r="L47">
+        <v>25</v>
+      </c>
+      <c r="M47">
+        <v>20</v>
+      </c>
+      <c r="N47">
+        <v>11</v>
+      </c>
+      <c r="O47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>43555</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>50</v>
+      </c>
+      <c r="D48">
+        <v>48</v>
+      </c>
+      <c r="E48">
+        <v>34</v>
+      </c>
+      <c r="F48">
+        <v>36</v>
+      </c>
+      <c r="G48">
+        <v>12</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>75</v>
+      </c>
+      <c r="K48">
+        <v>27</v>
+      </c>
+      <c r="L48">
+        <v>25</v>
+      </c>
+      <c r="M48">
+        <v>20</v>
+      </c>
+      <c r="N48">
+        <v>11</v>
+      </c>
+      <c r="O48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>43556</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49">
+        <v>48</v>
+      </c>
+      <c r="E49">
+        <v>34</v>
+      </c>
+      <c r="F49">
+        <v>36</v>
+      </c>
+      <c r="G49">
+        <v>12</v>
+      </c>
+      <c r="H49">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
         <v>74</v>
       </c>
-      <c r="K42">
+      <c r="K49">
         <v>28</v>
       </c>
-      <c r="L42">
-        <v>25</v>
-      </c>
-      <c r="M42">
+      <c r="L49">
+        <v>25</v>
+      </c>
+      <c r="M49">
         <v>20</v>
       </c>
-      <c r="N42">
-        <v>11</v>
-      </c>
-      <c r="O42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="A43" s="1">
+      <c r="N49">
+        <v>11</v>
+      </c>
+      <c r="O49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>43557</v>
       </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43">
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
         <v>52</v>
       </c>
-      <c r="D43">
+      <c r="D50">
         <v>58</v>
       </c>
-      <c r="E43">
+      <c r="E50">
         <v>42</v>
       </c>
-      <c r="F43">
+      <c r="F50">
         <v>43</v>
       </c>
-      <c r="G43">
+      <c r="G50">
         <v>12</v>
       </c>
-      <c r="H43">
+      <c r="H50">
         <v>5</v>
       </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
         <v>76</v>
       </c>
-      <c r="K43">
+      <c r="K50">
         <v>30</v>
       </c>
-      <c r="L43">
+      <c r="L50">
         <v>27</v>
       </c>
-      <c r="M43">
+      <c r="M50">
         <v>22</v>
       </c>
-      <c r="N43">
-        <v>11</v>
-      </c>
-      <c r="O43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="A44" s="1">
+      <c r="N50">
+        <v>11</v>
+      </c>
+      <c r="O50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>43558</v>
       </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44">
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
         <v>56</v>
       </c>
-      <c r="D44">
+      <c r="D51">
         <v>68</v>
       </c>
-      <c r="E44">
+      <c r="E51">
         <v>62</v>
       </c>
-      <c r="F44">
+      <c r="F51">
         <v>50</v>
       </c>
-      <c r="G44">
+      <c r="G51">
         <v>14</v>
       </c>
-      <c r="H44">
+      <c r="H51">
         <v>5</v>
       </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
         <v>78</v>
       </c>
-      <c r="K44">
+      <c r="K51">
         <v>33</v>
       </c>
-      <c r="L44">
+      <c r="L51">
         <v>31</v>
       </c>
-      <c r="M44">
-        <v>25</v>
-      </c>
-      <c r="N44">
+      <c r="M51">
+        <v>25</v>
+      </c>
+      <c r="N51">
         <v>12</v>
       </c>
-      <c r="O44">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" s="1">
+      <c r="O51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>43559</v>
       </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45">
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
         <v>57</v>
       </c>
-      <c r="D45">
+      <c r="D52">
         <v>70</v>
       </c>
-      <c r="E45">
+      <c r="E52">
         <v>72</v>
       </c>
-      <c r="F45">
+      <c r="F52">
         <v>54</v>
       </c>
-      <c r="G45">
+      <c r="G52">
         <v>14</v>
       </c>
-      <c r="H45">
+      <c r="H52">
         <v>5</v>
       </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
         <v>78</v>
       </c>
-      <c r="K45">
+      <c r="K52">
         <v>33</v>
       </c>
-      <c r="L45">
+      <c r="L52">
         <v>33</v>
       </c>
-      <c r="M45">
-        <v>25</v>
-      </c>
-      <c r="N45">
+      <c r="M52">
+        <v>25</v>
+      </c>
+      <c r="N52">
         <v>12</v>
       </c>
-      <c r="O45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15">
-      <c r="A46" s="1">
+      <c r="O52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>43560</v>
       </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="C46">
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
         <v>57</v>
       </c>
-      <c r="D46">
+      <c r="D53">
         <v>72</v>
       </c>
-      <c r="E46">
+      <c r="E53">
         <v>74</v>
       </c>
-      <c r="F46">
+      <c r="F53">
         <v>56</v>
       </c>
-      <c r="G46">
+      <c r="G53">
         <v>14</v>
       </c>
-      <c r="H46">
+      <c r="H53">
         <v>5</v>
       </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-      <c r="J46">
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
         <v>78</v>
       </c>
-      <c r="K46">
+      <c r="K53">
         <v>34</v>
       </c>
-      <c r="L46">
+      <c r="L53">
         <v>33</v>
       </c>
-      <c r="M46">
-        <v>25</v>
-      </c>
-      <c r="N46">
+      <c r="M53">
+        <v>25</v>
+      </c>
+      <c r="N53">
         <v>12</v>
       </c>
-      <c r="O46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="A47" s="1">
+      <c r="O53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
         <v>43561</v>
       </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
-      <c r="C47">
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
         <v>57</v>
       </c>
-      <c r="D47">
+      <c r="D54">
         <v>72</v>
       </c>
-      <c r="E47">
+      <c r="E54">
         <v>75</v>
       </c>
-      <c r="F47">
+      <c r="F54">
         <v>57</v>
       </c>
-      <c r="G47">
+      <c r="G54">
         <v>14</v>
       </c>
-      <c r="H47">
+      <c r="H54">
         <v>5</v>
       </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-      <c r="J47">
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
         <v>78</v>
       </c>
-      <c r="K47">
+      <c r="K54">
         <v>34</v>
       </c>
-      <c r="L47">
+      <c r="L54">
         <v>34</v>
       </c>
-      <c r="M47">
-        <v>25</v>
-      </c>
-      <c r="N47">
+      <c r="M54">
+        <v>25</v>
+      </c>
+      <c r="N54">
         <v>12</v>
       </c>
-      <c r="O47">
+      <c r="O54">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>